<commit_message>
Adding more info to testing docs
</commit_message>
<xml_diff>
--- a/Testing/Wind tunnel/23rd Sept/Wind tunnel test 23Sept - Funnel inlet.xlsx
+++ b/Testing/Wind tunnel/23rd Sept/Wind tunnel test 23Sept - Funnel inlet.xlsx
@@ -22476,16 +22476,16 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>2</xdr:col>
-      <xdr:colOff>209549</xdr:colOff>
-      <xdr:row>2</xdr:row>
-      <xdr:rowOff>47625</xdr:rowOff>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>266699</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>133350</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>15</xdr:col>
-      <xdr:colOff>276225</xdr:colOff>
-      <xdr:row>35</xdr:row>
-      <xdr:rowOff>123825</xdr:rowOff>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>447675</xdr:colOff>
+      <xdr:row>34</xdr:row>
+      <xdr:rowOff>19050</xdr:rowOff>
     </xdr:to>
     <xdr:grpSp>
       <xdr:nvGrpSpPr>
@@ -22494,7 +22494,7 @@
       </xdr:nvGrpSpPr>
       <xdr:grpSpPr>
         <a:xfrm>
-          <a:off x="1924049" y="428625"/>
+          <a:off x="266699" y="133350"/>
           <a:ext cx="9925051" cy="6362700"/>
           <a:chOff x="5610224" y="381000"/>
           <a:chExt cx="9925051" cy="6362700"/>
@@ -22981,16 +22981,16 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>16</xdr:col>
-      <xdr:colOff>285750</xdr:colOff>
-      <xdr:row>7</xdr:row>
-      <xdr:rowOff>180975</xdr:rowOff>
+      <xdr:col>14</xdr:col>
+      <xdr:colOff>571500</xdr:colOff>
+      <xdr:row>2</xdr:row>
+      <xdr:rowOff>85725</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>19</xdr:col>
-      <xdr:colOff>600075</xdr:colOff>
-      <xdr:row>16</xdr:row>
-      <xdr:rowOff>38100</xdr:rowOff>
+      <xdr:col>18</xdr:col>
+      <xdr:colOff>276225</xdr:colOff>
+      <xdr:row>10</xdr:row>
+      <xdr:rowOff>133350</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
@@ -22999,7 +22999,7 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="12468225" y="1514475"/>
+          <a:off x="11534775" y="466725"/>
           <a:ext cx="2143125" cy="1571625"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
@@ -23043,6 +23043,299 @@
             <a:t> the concentration is closest to what is expected with the lid on at 20° forward &gt;&gt; best funnel configuration.</a:t>
           </a:r>
           <a:endParaRPr lang="en-NZ" sz="1400"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>19</xdr:col>
+      <xdr:colOff>180975</xdr:colOff>
+      <xdr:row>1</xdr:row>
+      <xdr:rowOff>57150</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>23</xdr:col>
+      <xdr:colOff>514350</xdr:colOff>
+      <xdr:row>12</xdr:row>
+      <xdr:rowOff>133350</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="17" name="TextBox 16"/>
+        <xdr:cNvSpPr txBox="1"/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="14192250" y="247650"/>
+          <a:ext cx="2771775" cy="2171700"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:schemeClr val="lt1"/>
+        </a:solidFill>
+        <a:ln w="9525" cmpd="sng">
+          <a:solidFill>
+            <a:schemeClr val="lt1">
+              <a:shade val="50000"/>
+            </a:schemeClr>
+          </a:solidFill>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="dk1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="square" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-NZ" sz="1600" u="sng">
+              <a:solidFill>
+                <a:srgbClr val="FF0000"/>
+              </a:solidFill>
+            </a:rPr>
+            <a:t>Testing Parameters:</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-NZ" sz="1600" u="none" baseline="0">
+              <a:solidFill>
+                <a:srgbClr val="FF0000"/>
+              </a:solidFill>
+            </a:rPr>
+            <a:t>-5m/s airspeed</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:pPr marL="0" marR="0" indent="0" defTabSz="914400" eaLnBrk="1" fontAlgn="auto" latinLnBrk="0" hangingPunct="1">
+            <a:lnSpc>
+              <a:spcPct val="100000"/>
+            </a:lnSpc>
+            <a:spcBef>
+              <a:spcPts val="0"/>
+            </a:spcBef>
+            <a:spcAft>
+              <a:spcPts val="0"/>
+            </a:spcAft>
+            <a:buClrTx/>
+            <a:buSzTx/>
+            <a:buFontTx/>
+            <a:buNone/>
+            <a:tabLst/>
+            <a:defRPr/>
+          </a:pPr>
+          <a:r>
+            <a:rPr lang="en-NZ" sz="1600">
+              <a:solidFill>
+                <a:srgbClr val="FF0000"/>
+              </a:solidFill>
+              <a:effectLst/>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t>-Mt.</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-NZ" sz="1600" baseline="0">
+              <a:solidFill>
+                <a:srgbClr val="FF0000"/>
+              </a:solidFill>
+              <a:effectLst/>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t> Bromo ash, sieved to &lt;53 micron</a:t>
+          </a:r>
+          <a:endParaRPr lang="en-NZ" sz="1600" u="none" baseline="0">
+            <a:solidFill>
+              <a:srgbClr val="FF0000"/>
+            </a:solidFill>
+          </a:endParaRPr>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-NZ" sz="1600" u="none" baseline="0">
+              <a:solidFill>
+                <a:srgbClr val="FF0000"/>
+              </a:solidFill>
+            </a:rPr>
+            <a:t>-SAG with 3.3% belt speed to give 30 g/hour flow to give approx 10 mg/m^3 ash/air concentration.</a:t>
+          </a:r>
+          <a:endParaRPr lang="en-NZ" sz="1600" u="none">
+            <a:solidFill>
+              <a:srgbClr val="FF0000"/>
+            </a:solidFill>
+          </a:endParaRPr>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>104775</xdr:colOff>
+      <xdr:row>13</xdr:row>
+      <xdr:rowOff>133350</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>18</xdr:col>
+      <xdr:colOff>580725</xdr:colOff>
+      <xdr:row>25</xdr:row>
+      <xdr:rowOff>76200</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="18" name="Picture 17"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId2"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="10458450" y="2609850"/>
+          <a:ext cx="3523950" cy="2228850"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>85725</xdr:colOff>
+      <xdr:row>26</xdr:row>
+      <xdr:rowOff>114300</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>19</xdr:col>
+      <xdr:colOff>30068</xdr:colOff>
+      <xdr:row>42</xdr:row>
+      <xdr:rowOff>66675</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="19" name="Picture 18"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill rotWithShape="1">
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId3"/>
+        <a:srcRect l="6541" r="5430"/>
+        <a:stretch/>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="10439400" y="5067300"/>
+          <a:ext cx="3601943" cy="3000375"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>19</xdr:col>
+      <xdr:colOff>419100</xdr:colOff>
+      <xdr:row>17</xdr:row>
+      <xdr:rowOff>57150</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>24</xdr:col>
+      <xdr:colOff>114300</xdr:colOff>
+      <xdr:row>24</xdr:row>
+      <xdr:rowOff>19050</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="20" name="TextBox 19"/>
+        <xdr:cNvSpPr txBox="1"/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="14430375" y="3295650"/>
+          <a:ext cx="2743200" cy="1295400"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:schemeClr val="lt1"/>
+        </a:solidFill>
+        <a:ln w="9525" cmpd="sng">
+          <a:solidFill>
+            <a:schemeClr val="lt1">
+              <a:shade val="50000"/>
+            </a:schemeClr>
+          </a:solidFill>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="dk1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="square" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-NZ" sz="1600"/>
+            <a:t>Testing done in configuration</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-NZ" sz="1600" baseline="0"/>
+            <a:t> shown</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-NZ" sz="1600"/>
+            <a:t> </a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-NZ" sz="1600" baseline="0"/>
+            <a:t>left, funnel inlet angle was changed by pitching it forwards and backwards.</a:t>
+          </a:r>
+          <a:endParaRPr lang="en-NZ" sz="1600"/>
         </a:p>
       </xdr:txBody>
     </xdr:sp>
@@ -24405,7 +24698,7 @@
   <dimension ref="A1:I388"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="S19" sqref="S19"/>
+      <selection activeCell="V30" sqref="V30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>